<commit_message>
nomina: actualización de plantilla para subir banco y cuenta banco
</commit_message>
<xml_diff>
--- a/extras/plantilla_empleados.xlsx
+++ b/extras/plantilla_empleados.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>SEDE</t>
   </si>
@@ -195,6 +195,12 @@
   </si>
   <si>
     <t>PAGO_SUELDO_NETO</t>
+  </si>
+  <si>
+    <t>BANCO</t>
+  </si>
+  <si>
+    <t>CUENTA_BANCO</t>
   </si>
 </sst>
 </file>
@@ -524,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE1"/>
+  <dimension ref="A1:AG1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -554,18 +560,20 @@
     <col min="20" max="20" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="18" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="38.5" customWidth="1"/>
-    <col min="30" max="30" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="38.5" customWidth="1"/>
+    <col min="32" max="32" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -633,30 +641,36 @@
         <v>21</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>